<commit_message>
Refine Fig3C zoomed plot and legend positioning
Updated the zoomed-in version of the Fig3C gradient plot to exclude the first two and last two fractions and to remove EZH2 for clarity. Adjusted the legend positioning to use the new 'legend.position.inside' parameter and improved axis and theme settings for better visualization.
</commit_message>
<xml_diff>
--- a/_Manuscript/Supplementary_Tables/Supplementary_Table_2.xlsx
+++ b/_Manuscript/Supplementary_Tables/Supplementary_Table_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28019"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niar/OneDrive - CRG - Centre de Regulacio Genomica/Suz12_AS_project/_Manuscript/Supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7610AC-2074-724E-A2E6-1A144A072CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7610AC-2074-724E-A2E6-1A144A072CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29140" yWindow="2540" windowWidth="24760" windowHeight="18500" xr2:uid="{C863A306-5043-D543-A8AC-8BA276D7CE67}"/>
   </bookViews>
   <sheets>
     <sheet name="Oligos-primers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,48 +38,84 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
+    <t>PSI validation</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Sequence (5'-3')</t>
   </si>
   <si>
+    <t>human Suz12 ex3-5 Fw</t>
+  </si>
+  <si>
     <t>CCAATATTTTTGCACAGAACTCTTAC</t>
   </si>
   <si>
+    <t>human Suz12 ex3-5 Rv</t>
+  </si>
+  <si>
     <t>TTTGTGGAAGAAACCAGTAAACGT</t>
   </si>
   <si>
+    <t>mouse Suz12 ex3-5 Fw</t>
+  </si>
+  <si>
+    <t>mouse Suz12 ex3-5 Rv</t>
+  </si>
+  <si>
     <t>CATTTTTGTGGAAGAAACCGGT</t>
   </si>
   <si>
+    <t>zebrafish Suz12a ex3-5 Fw</t>
+  </si>
+  <si>
     <t>CCAATTTTCCTGCACCGATCT</t>
   </si>
   <si>
+    <t>zebrafish Suz12a ex3-5 Rv</t>
+  </si>
+  <si>
     <t>GGAAGAATCCAGTGAAAGTGAGT</t>
   </si>
   <si>
-    <t>PSI validation</t>
-  </si>
-  <si>
     <t>RT-qPCR</t>
   </si>
   <si>
+    <t>mouse Suz12 Fw</t>
+  </si>
+  <si>
     <t>GTGCACTCTGAACTGCCGTA</t>
   </si>
   <si>
+    <t>mouse Suz12 Rv</t>
+  </si>
+  <si>
     <t>CCGGTCCATTTCGACTAAAA</t>
   </si>
   <si>
+    <t>mouse Ezh2 Fw</t>
+  </si>
+  <si>
     <t>AAGACTATGTTTAGTTCCAATCGTCAG</t>
   </si>
   <si>
+    <t>mouse Ezh2 Rv</t>
+  </si>
+  <si>
     <t>TCACTGGTGACTGAACAAGAAGTC</t>
   </si>
   <si>
+    <t>mouse Nanog Fw</t>
+  </si>
+  <si>
     <t>CTTACAAGGGTCTGCTACTGAGATGC</t>
   </si>
   <si>
+    <t>mouse Nanog Rv</t>
+  </si>
+  <si>
     <t>TGCTTCCTGGCAAGGACCTT</t>
   </si>
   <si>
@@ -138,6 +179,9 @@
     <t>GCCCCCATCGCTGCACAAAATA</t>
   </si>
   <si>
+    <t>Mouse ChIP-qPCR</t>
+  </si>
+  <si>
     <t>Gsc prom Fw</t>
   </si>
   <si>
@@ -208,52 +252,13 @@
   </si>
   <si>
     <t>GAAGTGCAATTGGGATGAAAA</t>
-  </si>
-  <si>
-    <t>Mouse ChIP-qPCR</t>
-  </si>
-  <si>
-    <t>human Suz12 ex3-5 Fw</t>
-  </si>
-  <si>
-    <t>human Suz12 ex3-5 Rv</t>
-  </si>
-  <si>
-    <t>mouse Suz12 ex3-5 Fw</t>
-  </si>
-  <si>
-    <t>mouse Suz12 ex3-5 Rv</t>
-  </si>
-  <si>
-    <t>zebrafish Suz12a ex3-5 Fw</t>
-  </si>
-  <si>
-    <t>zebrafish Suz12a ex3-5 Rv</t>
-  </si>
-  <si>
-    <t>mouse Suz12 Fw</t>
-  </si>
-  <si>
-    <t>mouse Suz12 Rv</t>
-  </si>
-  <si>
-    <t>mouse Ezh2 Fw</t>
-  </si>
-  <si>
-    <t>mouse Ezh2 Rv</t>
-  </si>
-  <si>
-    <t>mouse Nanog Fw</t>
-  </si>
-  <si>
-    <t>mouse Nanog Rv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,10 +318,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,360 +642,360 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>